<commit_message>
add tain topic law-why
</commit_message>
<xml_diff>
--- a/chat_bot/data/tain_law.xlsx
+++ b/chat_bot/data/tain_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="109">
   <si>
     <t>tag</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>ยื่นเสียภาษีตอนเงินเดือนกี่บาท</t>
+  </si>
+  <si>
+    <t>เก็บภาษีทำไม</t>
+  </si>
+  <si>
+    <t>เก็บภาษีเพื่อ</t>
   </si>
 </sst>
 </file>
@@ -674,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="79" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="79" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1194,15 +1200,15 @@
         <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2">
-      <c r="A65" t="s">
-        <v>73</v>
+      <c r="A65" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1210,7 +1216,7 @@
         <v>73</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1218,7 +1224,7 @@
         <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1226,7 +1232,7 @@
         <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1234,7 +1240,7 @@
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1242,7 +1248,7 @@
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1250,7 +1256,7 @@
         <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1258,7 +1264,7 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1266,15 +1272,15 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1282,7 +1288,7 @@
         <v>83</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1290,7 +1296,7 @@
         <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1298,7 +1304,7 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1306,7 +1312,7 @@
         <v>83</v>
       </c>
       <c r="B78" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1314,7 +1320,7 @@
         <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1322,7 +1328,7 @@
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1330,7 +1336,7 @@
         <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1338,15 +1344,15 @@
         <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1354,7 +1360,7 @@
         <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1362,7 +1368,7 @@
         <v>93</v>
       </c>
       <c r="B85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1370,7 +1376,7 @@
         <v>93</v>
       </c>
       <c r="B86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1378,7 +1384,7 @@
         <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1386,7 +1392,7 @@
         <v>93</v>
       </c>
       <c r="B88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1394,15 +1400,15 @@
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1410,7 +1416,7 @@
         <v>101</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1418,7 +1424,7 @@
         <v>101</v>
       </c>
       <c r="B92" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1426,7 +1432,7 @@
         <v>101</v>
       </c>
       <c r="B93" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1434,6 +1440,14 @@
         <v>101</v>
       </c>
       <c r="B94" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="B95" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit data for train bot
</commit_message>
<xml_diff>
--- a/chat_bot/data/tain_law.xlsx
+++ b/chat_bot/data/tain_law.xlsx
@@ -41,9 +41,6 @@
     <t>สวัสดีครับ</t>
   </si>
   <si>
-    <t>สวัสดีคะ</t>
-  </si>
-  <si>
     <t>หวัดดี</t>
   </si>
   <si>
@@ -351,6 +348,9 @@
   </si>
   <si>
     <t>เก็บภาษีเพื่อ</t>
+  </si>
+  <si>
+    <t>สวัสดีค่ะ</t>
   </si>
 </sst>
 </file>
@@ -682,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="79" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -720,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -728,7 +728,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -736,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -744,7 +744,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -752,703 +752,703 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="28.5">
       <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="28.5">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="28.5">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.5">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="28.5">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="28.5">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="28.5">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.5">
       <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="28.5">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="28.5">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="28.5">
       <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="28.5">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="28.5">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="28.5">
       <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="28.5">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="28.5">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="28.5">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28.5">
       <c r="A26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="28.5">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="28.5">
       <c r="A28" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="28.5">
       <c r="A29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="28.5">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="28.5">
       <c r="A31" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="28.5">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="28.5">
       <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="28.5">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="28.5">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.5">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="28.5">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="28.5">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="28.5">
       <c r="A47" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="28.5">
       <c r="A48" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="28.5">
       <c r="A49" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="28.5">
       <c r="A50" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55" t="s">
         <v>49</v>
-      </c>
-      <c r="B55" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="s">
         <v>66</v>
-      </c>
-      <c r="B58" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B66" t="s">
         <v>73</v>
-      </c>
-      <c r="B66" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" t="s">
         <v>83</v>
-      </c>
-      <c r="B75" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" t="s">
         <v>93</v>
-      </c>
-      <c r="B84" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91" t="s">
         <v>101</v>
-      </c>
-      <c r="B91" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B94" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B95" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add question about time to open page
</commit_message>
<xml_diff>
--- a/chat_bot/data/tain_law.xlsx
+++ b/chat_bot/data/tain_law.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="120">
   <si>
     <t>tag</t>
   </si>
@@ -366,6 +366,24 @@
   </si>
   <si>
     <t>จ่ายภาษีไหน</t>
+  </si>
+  <si>
+    <t>time-page</t>
+  </si>
+  <si>
+    <t>เวลาทำการของเพจ</t>
+  </si>
+  <si>
+    <t>เวลาของเพจ</t>
+  </si>
+  <si>
+    <t>เพจเปิดตอนไหน</t>
+  </si>
+  <si>
+    <t>เพจเปิดตีเท่าไหร่</t>
+  </si>
+  <si>
+    <t>เวลาเพจเปิด</t>
   </si>
 </sst>
 </file>
@@ -695,14 +713,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="79" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="37.75" customWidth="1"/>
   </cols>
   <sheetData>
@@ -794,148 +813,148 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.5">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="28.5">
+        <v>114</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="28.5">
+        <v>114</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="28.5">
+        <v>114</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="28.5">
+        <v>114</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.5">
+        <v>114</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="28.5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="28.5">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="28.5">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="28.5">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="28.5">
-      <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="28.5">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="28.5">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="28.5">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="28.5">
-      <c r="A26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="28.5">
-      <c r="A27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="28.5">
-      <c r="A28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="28.5">
-      <c r="A29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="28.5">
@@ -943,7 +962,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="28.5">
@@ -951,7 +970,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="28.5">
@@ -959,215 +978,215 @@
         <v>23</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="28.5">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="28.5">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="28.5">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="28.5">
       <c r="A36" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.5">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="28.5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="28.5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B49" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="28.5">
-      <c r="A48" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="28.5">
-      <c r="A49" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="28.5">
-      <c r="A50" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="28.5">
-      <c r="A51" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B51" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="28.5">
-      <c r="A52" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B52" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="28.5">
+    <row r="53" spans="1:2">
       <c r="A53" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B53" t="s">
-        <v>61</v>
+      <c r="B53" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1175,7 +1194,7 @@
         <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1183,47 +1202,47 @@
         <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1231,7 +1250,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1239,7 +1258,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1247,47 +1266,47 @@
         <v>65</v>
       </c>
       <c r="B68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B73" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1295,7 +1314,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1303,7 +1322,7 @@
         <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1311,7 +1330,7 @@
         <v>72</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1319,47 +1338,47 @@
         <v>72</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B78" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B82" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1367,7 +1386,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1375,7 +1394,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1383,7 +1402,7 @@
         <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1391,47 +1410,47 @@
         <v>82</v>
       </c>
       <c r="B86" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1439,7 +1458,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1447,7 +1466,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1455,7 +1474,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1463,46 +1482,86 @@
         <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B96" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B98" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B99" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
+        <v>92</v>
+      </c>
+      <c r="B100" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>